<commit_message>
19/4 Lsg vs Csk
</commit_message>
<xml_diff>
--- a/frontend/public/Apr16.xlsx
+++ b/frontend/public/Apr16.xlsx
@@ -404,76 +404,76 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Rohit Sharma</v>
+        <v>KL Rahul</v>
       </c>
       <c r="B3" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C3" t="str">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Jasprit Bumrah</v>
+        <v>Rohit Sharma</v>
       </c>
       <c r="B4" t="str">
         <v>MI</v>
       </c>
       <c r="C4" t="str">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Sam Curran</v>
+        <v>Jasprit Bumrah</v>
       </c>
       <c r="B5" t="str">
-        <v>PBKS</v>
+        <v>MI</v>
       </c>
       <c r="C5" t="str">
-        <v>224</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Dinesh Karthik</v>
+        <v>Sam Curran</v>
       </c>
       <c r="B6" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C6" t="str">
-        <v>204</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Ashutosh Sharma</v>
+        <v>Ruturaj Gaikwad</v>
       </c>
       <c r="B7" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C7" t="str">
-        <v>201</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Ishan Kishan</v>
+        <v>Ashutosh Sharma</v>
       </c>
       <c r="B8" t="str">
-        <v>MI</v>
+        <v>PBKS</v>
       </c>
       <c r="C8" t="str">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Riyan Parag</v>
+        <v>Ishan Kishan</v>
       </c>
       <c r="B9" t="str">
-        <v>RR</v>
+        <v>MI</v>
       </c>
       <c r="C9" t="str">
         <v>199</v>
@@ -481,54 +481,54 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Ruturaj Gaikwad</v>
+        <v>Dinesh Karthik</v>
       </c>
       <c r="B10" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C10" t="str">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Suryakumar Yadav</v>
+        <v>Ravindra Jadeja</v>
       </c>
       <c r="B11" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C11" t="str">
-        <v>190</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Kuldeep Sen</v>
+        <v>Riyan Parag</v>
       </c>
       <c r="B12" t="str">
         <v>RR</v>
       </c>
       <c r="C12" t="str">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Harshal Patel</v>
+        <v>Kuldeep Sen</v>
       </c>
       <c r="B13" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C13" t="str">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Faf du Plessis</v>
+        <v>Suryakumar Yadav</v>
       </c>
       <c r="B14" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C14" t="str">
         <v>190</v>
@@ -536,142 +536,142 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Travis Head</v>
+        <v>Faf du Plessis</v>
       </c>
       <c r="B15" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C15" t="str">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Jos Buttler</v>
+        <v>Harshal Patel</v>
       </c>
       <c r="B16" t="str">
-        <v>RR</v>
+        <v>PBKS</v>
       </c>
       <c r="C16" t="str">
-        <v>172</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Sanju Samson</v>
+        <v>Shashank Singh</v>
       </c>
       <c r="B17" t="str">
-        <v>RR</v>
+        <v>PBKS</v>
       </c>
       <c r="C17" t="str">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Avesh Khan</v>
+        <v>Travis Head</v>
       </c>
       <c r="B18" t="str">
-        <v>RR</v>
+        <v>SRH</v>
       </c>
       <c r="C18" t="str">
-        <v>153</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Kagiso Rabada</v>
+        <v>Jos Buttler</v>
       </c>
       <c r="B19" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C19" t="str">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Shashank Singh</v>
+        <v>Philip Salt</v>
       </c>
       <c r="B20" t="str">
-        <v>PBKS</v>
+        <v>KKR</v>
       </c>
       <c r="C20" t="str">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Pat Cummins</v>
+        <v>Sanju Samson</v>
       </c>
       <c r="B21" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C21" t="str">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Philip Salt</v>
+        <v>Kagiso Rabada</v>
       </c>
       <c r="B22" t="str">
-        <v>KKR</v>
+        <v>PBKS</v>
       </c>
       <c r="C22" t="str">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Heinrich Klaasen</v>
+        <v>Avesh Khan</v>
       </c>
       <c r="B23" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C23" t="str">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Gerald Coetzee</v>
+        <v>Heinrich Klaasen</v>
       </c>
       <c r="B24" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C24" t="str">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Rishabh Pant</v>
+        <v>Matheesha Pathirana</v>
       </c>
       <c r="B25" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C25" t="str">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Shivam Dube</v>
+        <v>Pat Cummins</v>
       </c>
       <c r="B26" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C26" t="str">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Tilak Varma</v>
+        <v>Arshdeep Singh</v>
       </c>
       <c r="B27" t="str">
-        <v>MI</v>
+        <v>PBKS</v>
       </c>
       <c r="C27" t="str">
         <v>137</v>
@@ -679,65 +679,65 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Nithish Reddy</v>
+        <v>Gerald Coetzee</v>
       </c>
       <c r="B28" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C28" t="str">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>KL Rahul</v>
+        <v>Rishabh Pant</v>
       </c>
       <c r="B29" t="str">
-        <v>LSG</v>
+        <v>DC</v>
       </c>
       <c r="C29" t="str">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Arshdeep Singh</v>
+        <v>Shivam Dube</v>
       </c>
       <c r="B30" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C30" t="str">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Rashid Khan</v>
+        <v>Tilak Varma</v>
       </c>
       <c r="B31" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C31" t="str">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Shreyas Iyer</v>
+        <v>Rashid Khan</v>
       </c>
       <c r="B32" t="str">
-        <v>KKR</v>
+        <v>GT</v>
       </c>
       <c r="C32" t="str">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Mukesh Kumar</v>
+        <v>Hardik Pandya</v>
       </c>
       <c r="B33" t="str">
-        <v>DC</v>
+        <v>MI</v>
       </c>
       <c r="C33" t="str">
         <v>130</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Hardik Pandya</v>
+        <v>Mukesh Kumar</v>
       </c>
       <c r="B34" t="str">
-        <v>MI</v>
+        <v>DC</v>
       </c>
       <c r="C34" t="str">
         <v>130</v>
@@ -756,13 +756,13 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Ravindra Jadeja</v>
+        <v>Shreyas Iyer</v>
       </c>
       <c r="B35" t="str">
-        <v>CSK</v>
+        <v>KKR</v>
       </c>
       <c r="C35" t="str">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36">
@@ -773,26 +773,26 @@
         <v>LSG</v>
       </c>
       <c r="C36" t="str">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Yuzvendra Chahal</v>
+        <v>Tushar Deshpande</v>
       </c>
       <c r="B37" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C37" t="str">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Matheesha Pathirana</v>
+        <v>Yuzvendra Chahal</v>
       </c>
       <c r="B38" t="str">
-        <v>CSK</v>
+        <v>RR</v>
       </c>
       <c r="C38" t="str">
         <v>120</v>
@@ -800,428 +800,428 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Khaleel Ahmed</v>
+        <v>Quinton de Kock</v>
       </c>
       <c r="B39" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C39" t="str">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Yashasvi Jaiswal</v>
+        <v>Mustafizur Rahman</v>
       </c>
       <c r="B40" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C40" t="str">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Tushar Deshpande</v>
+        <v>Khaleel Ahmed</v>
       </c>
       <c r="B41" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C41" t="str">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Shubman Gill</v>
+        <v>Yashasvi Jaiswal</v>
       </c>
       <c r="B42" t="str">
-        <v>GT</v>
+        <v>RR</v>
       </c>
       <c r="C42" t="str">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Jitesh Sharma</v>
+        <v>Nicholas Pooran</v>
       </c>
       <c r="B43" t="str">
-        <v>PBKS</v>
+        <v>LSG</v>
       </c>
       <c r="C43" t="str">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Kuldeep Yadav</v>
+        <v>Shubman Gill</v>
       </c>
       <c r="B44" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C44" t="str">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Abdul Samad</v>
+        <v>Vaibhav Arora</v>
       </c>
       <c r="B45" t="str">
-        <v>SRH</v>
+        <v>KKR</v>
       </c>
       <c r="C45" t="str">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Mitchell Starc</v>
+        <v>Nithish Reddy</v>
       </c>
       <c r="B46" t="str">
-        <v>KKR</v>
+        <v>SRH</v>
       </c>
       <c r="C46" t="str">
-        <v>99</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Angkrish Raghuvanshi</v>
+        <v>Jitesh Sharma</v>
       </c>
       <c r="B47" t="str">
-        <v>KKR</v>
+        <v>PBKS</v>
       </c>
       <c r="C47" t="str">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Shreyas Gopal</v>
+        <v>Kuldeep Yadav</v>
       </c>
       <c r="B48" t="str">
-        <v>MI</v>
+        <v>DC</v>
       </c>
       <c r="C48" t="str">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Ishant Sharma</v>
+        <v>Abdul Samad</v>
       </c>
       <c r="B49" t="str">
-        <v>DC</v>
+        <v>SRH</v>
       </c>
       <c r="C49" t="str">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Rajat Patidar</v>
+        <v>Mitchell Starc</v>
       </c>
       <c r="B50" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C50" t="str">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Mustafizur Rahman</v>
+        <v>Varun Chakravarthy</v>
       </c>
       <c r="B51" t="str">
-        <v>CSK</v>
+        <v>KKR</v>
       </c>
       <c r="C51" t="str">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Abhishek Sharma</v>
+        <v>Shreyas Gopal</v>
       </c>
       <c r="B52" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C52" t="str">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Virat Kohli</v>
+        <v>Angkrish Raghuvanshi</v>
       </c>
       <c r="B53" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C53" t="str">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Trent Boult</v>
+        <v>Ishant Sharma</v>
       </c>
       <c r="B54" t="str">
-        <v>RR</v>
+        <v>DC</v>
       </c>
       <c r="C54" t="str">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Liam Livingstone</v>
+        <v>Rajat Patidar</v>
       </c>
       <c r="B55" t="str">
-        <v>PBKS</v>
+        <v>RCB</v>
       </c>
       <c r="C55" t="str">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Varun Chakravarthy</v>
+        <v>Mohsin Khan</v>
       </c>
       <c r="B56" t="str">
-        <v>KKR</v>
+        <v>LSG</v>
       </c>
       <c r="C56" t="str">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Vaibhav Arora</v>
+        <v>Ravi Bishnoi</v>
       </c>
       <c r="B57" t="str">
-        <v>KKR</v>
+        <v>LSG</v>
       </c>
       <c r="C57" t="str">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Nicholas Pooran</v>
+        <v>Virat Kohli</v>
       </c>
       <c r="B58" t="str">
-        <v>LSG</v>
+        <v>RCB</v>
       </c>
       <c r="C58" t="str">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Tristan Stubbs</v>
+        <v>Marcus Stoinis</v>
       </c>
       <c r="B59" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C59" t="str">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Shimron Hetmyer</v>
+        <v>Liam Livingstone</v>
       </c>
       <c r="B60" t="str">
-        <v>RR</v>
+        <v>PBKS</v>
       </c>
       <c r="C60" t="str">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Bhuvneshwar Kumar</v>
+        <v>Abhishek Sharma</v>
       </c>
       <c r="B61" t="str">
         <v>SRH</v>
       </c>
       <c r="C61" t="str">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Daryl Mitchell</v>
+        <v>Trent Boult</v>
       </c>
       <c r="B62" t="str">
-        <v>CSK</v>
+        <v>RR</v>
       </c>
       <c r="C62" t="str">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Prithvi Shaw</v>
+        <v>MS Dhoni</v>
       </c>
       <c r="B63" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C63" t="str">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>B Sai Sudharsan</v>
+        <v>Krunal Pandya</v>
       </c>
       <c r="B64" t="str">
-        <v>GT</v>
+        <v>LSG</v>
       </c>
       <c r="C64" t="str">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Andre Russell</v>
+        <v>Tristan Stubbs</v>
       </c>
       <c r="B65" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C65" t="str">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Ravi Bishnoi</v>
+        <v>Andre Russell</v>
       </c>
       <c r="B66" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C66" t="str">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Harpreet Brar</v>
+        <v>Shimron Hetmyer</v>
       </c>
       <c r="B67" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C67" t="str">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Mohammad Nabi</v>
+        <v>Daryl Mitchell</v>
       </c>
       <c r="B68" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C68" t="str">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Tim David</v>
+        <v>Rachin Ravindra</v>
       </c>
       <c r="B69" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C69" t="str">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Rachin Ravindra</v>
+        <v>Bhuvneshwar Kumar</v>
       </c>
       <c r="B70" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C70" t="str">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Dhruv Jurel</v>
+        <v>Ajinkya Rahane</v>
       </c>
       <c r="B71" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C71" t="str">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Mayank Markande</v>
+        <v>Prithvi Shaw</v>
       </c>
       <c r="B72" t="str">
-        <v>SRH</v>
+        <v>DC</v>
       </c>
       <c r="C72" t="str">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Rahul Tewatia</v>
+        <v>B Sai Sudharsan</v>
       </c>
       <c r="B73" t="str">
         <v>GT</v>
       </c>
       <c r="C73" t="str">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Lockie Ferguson</v>
+        <v>Tim David</v>
       </c>
       <c r="B74" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C74" t="str">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Aiden Markram</v>
+        <v>Harpreet Brar</v>
       </c>
       <c r="B75" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C75" t="str">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Harshit Rana</v>
+        <v>Mohammad Nabi</v>
       </c>
       <c r="B76" t="str">
-        <v>KKR</v>
+        <v>MI</v>
       </c>
       <c r="C76" t="str">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Akash Madhwal</v>
+        <v>Rovman Powell</v>
       </c>
       <c r="B77" t="str">
-        <v>MI</v>
+        <v>RR</v>
       </c>
       <c r="C77" t="str">
         <v>60</v>
@@ -1229,142 +1229,142 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>T Natarajan</v>
+        <v>Dhruv Jurel</v>
       </c>
       <c r="B78" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C78" t="str">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>Shai Hope</v>
+        <v>Akash Madhwal</v>
       </c>
       <c r="B79" t="str">
-        <v>DC</v>
+        <v>MI</v>
       </c>
       <c r="C79" t="str">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>Mohsin Khan</v>
+        <v>Yash Thakur</v>
       </c>
       <c r="B80" t="str">
         <v>LSG</v>
       </c>
       <c r="C80" t="str">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Rovman Powell</v>
+        <v>Mayank Markande</v>
       </c>
       <c r="B81" t="str">
-        <v>RR</v>
+        <v>SRH</v>
       </c>
       <c r="C81" t="str">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Axar Patel</v>
+        <v>Rahul Tewatia</v>
       </c>
       <c r="B82" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C82" t="str">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>Rinku Singh</v>
+        <v>Lockie Ferguson</v>
       </c>
       <c r="B83" t="str">
-        <v>KKR</v>
+        <v>RCB</v>
       </c>
       <c r="C83" t="str">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>Ramandeep Singh</v>
+        <v>Aiden Markram</v>
       </c>
       <c r="B84" t="str">
-        <v>KKR</v>
+        <v>SRH</v>
       </c>
       <c r="C84" t="str">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>Mahipal Lomror</v>
+        <v>Harshit Rana</v>
       </c>
       <c r="B85" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C85" t="str">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>Will Jacks</v>
+        <v>T Natarajan</v>
       </c>
       <c r="B86" t="str">
-        <v>RCB</v>
+        <v>SRH</v>
       </c>
       <c r="C86" t="str">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Maheesh Theekshana</v>
+        <v>Shai Hope</v>
       </c>
       <c r="B87" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C87" t="str">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>Sikandar Raza</v>
+        <v>Axar Patel</v>
       </c>
       <c r="B88" t="str">
-        <v>PBKS</v>
+        <v>DC</v>
       </c>
       <c r="C88" t="str">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>Anuj Rawat</v>
+        <v>Moeen Ali</v>
       </c>
       <c r="B89" t="str">
-        <v>RCB</v>
+        <v>CSK</v>
       </c>
       <c r="C89" t="str">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Quinton de Kock</v>
+        <v>Maheesh Theekshana</v>
       </c>
       <c r="B90" t="str">
-        <v>LSG</v>
+        <v>CSK</v>
       </c>
       <c r="C90" t="str">
         <v>45</v>
@@ -1372,244 +1372,244 @@
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Marcus Stoinis</v>
+        <v>Rinku Singh</v>
       </c>
       <c r="B91" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C91" t="str">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>Mohit Sharma</v>
+        <v>Ramandeep Singh</v>
       </c>
       <c r="B92" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C92" t="str">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Jack Fraser-Mcgurk</v>
+        <v>Mahipal Lomror</v>
       </c>
       <c r="B93" t="str">
-        <v>DC</v>
+        <v>RCB</v>
       </c>
       <c r="C93" t="str">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>Arshad Khan</v>
+        <v>Will Jacks</v>
       </c>
       <c r="B94" t="str">
-        <v>LSG</v>
+        <v>RCB</v>
       </c>
       <c r="C94" t="str">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>MS Dhoni</v>
+        <v>Jaydev Unadkat</v>
       </c>
       <c r="B95" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C95" t="str">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Vijay Shankar</v>
+        <v>Anuj Rawat</v>
       </c>
       <c r="B96" t="str">
-        <v>GT</v>
+        <v>RCB</v>
       </c>
       <c r="C96" t="str">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>Sumit Kumar</v>
+        <v>Sikandar Raza</v>
       </c>
       <c r="B97" t="str">
-        <v>DC</v>
+        <v>PBKS</v>
       </c>
       <c r="C97" t="str">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>Yash Thakur</v>
+        <v>Spencer Johnson</v>
       </c>
       <c r="B98" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C98" t="str">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Simran Singh</v>
+        <v>Mohit Sharma</v>
       </c>
       <c r="B99" t="str">
-        <v>PBKS</v>
+        <v>GT</v>
       </c>
       <c r="C99" t="str">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Vyshak Vijay Kumar</v>
+        <v>Jack Fraser-Mcgurk</v>
       </c>
       <c r="B100" t="str">
-        <v>RCB</v>
+        <v>DC</v>
       </c>
       <c r="C100" t="str">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>Jaydev Unadkat</v>
+        <v>Arshad Khan</v>
       </c>
       <c r="B101" t="str">
-        <v>SRH</v>
+        <v>LSG</v>
       </c>
       <c r="C101" t="str">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>Spencer Johnson</v>
+        <v>Vijay Shankar</v>
       </c>
       <c r="B102" t="str">
         <v>GT</v>
       </c>
       <c r="C102" t="str">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>Venkatesh Iyer</v>
+        <v>Sumit Kumar</v>
       </c>
       <c r="B103" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C103" t="str">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>Naveen-ul-Haq</v>
+        <v>Simran Singh</v>
       </c>
       <c r="B104" t="str">
-        <v>LSG</v>
+        <v>PBKS</v>
       </c>
       <c r="C104" t="str">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Shikhar Dhawan</v>
+        <v>Vyshak Vijay Kumar</v>
       </c>
       <c r="B105" t="str">
-        <v>PBKS</v>
+        <v>RCB</v>
       </c>
       <c r="C105" t="str">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>Deepak Hooda</v>
+        <v>Venkatesh Iyer</v>
       </c>
       <c r="B106" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C106" t="str">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Abhishek Porel</v>
+        <v>Deepak Hooda</v>
       </c>
       <c r="B107" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C107" t="str">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Umesh Yadav</v>
+        <v>Reece Topley</v>
       </c>
       <c r="B108" t="str">
-        <v>GT</v>
+        <v>RCB</v>
       </c>
       <c r="C108" t="str">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Reece Topley</v>
+        <v>Jonny Bairstow</v>
       </c>
       <c r="B109" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C109" t="str">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Jonny Bairstow</v>
+        <v>Naveen-ul-Haq</v>
       </c>
       <c r="B110" t="str">
-        <v>PBKS</v>
+        <v>LSG</v>
       </c>
       <c r="C110" t="str">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Shahbaz Ahmed</v>
+        <v>Shikhar Dhawan</v>
       </c>
       <c r="B111" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C111" t="str">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Shardul Thakur</v>
+        <v>Abhishek Porel</v>
       </c>
       <c r="B112" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C112" t="str">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="113">
@@ -1625,90 +1625,90 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>Shahrukh Khan</v>
+        <v>Umesh Yadav</v>
       </c>
       <c r="B114" t="str">
         <v>GT</v>
       </c>
       <c r="C114" t="str">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>Harpreet Singh</v>
+        <v>Shahbaz Ahmed</v>
       </c>
       <c r="B115" t="str">
-        <v>PBKS</v>
+        <v>SRH</v>
       </c>
       <c r="C115" t="str">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>Atharva Taide</v>
+        <v>Shardul Thakur</v>
       </c>
       <c r="B116" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C116" t="str">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>Abhinav Manohar</v>
+        <v>Shahrukh Khan</v>
       </c>
       <c r="B117" t="str">
         <v>GT</v>
       </c>
       <c r="C117" t="str">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>David Warner</v>
+        <v>Abhinav Manohar</v>
       </c>
       <c r="B118" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C118" t="str">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>Saurav Chauhan</v>
+        <v>David Warner</v>
       </c>
       <c r="B119" t="str">
-        <v>RCB</v>
+        <v>DC</v>
       </c>
       <c r="C119" t="str">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Rahul Tripathi</v>
+        <v>Harpreet Singh</v>
       </c>
       <c r="B120" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C120" t="str">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Matthew Wade</v>
+        <v>Atharva Taide</v>
       </c>
       <c r="B121" t="str">
-        <v>GT</v>
+        <v>PBKS</v>
       </c>
       <c r="C121" t="str">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122">
@@ -1724,54 +1724,54 @@
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>Ajinkya Rahane</v>
+        <v>Rahul Tripathi</v>
       </c>
       <c r="B123" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C123" t="str">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>Krunal Pandya</v>
+        <v>Matthew Wade</v>
       </c>
       <c r="B124" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C124" t="str">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>Sameer Rizvi</v>
+        <v>Saurav Chauhan</v>
       </c>
       <c r="B125" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C125" t="str">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>Noor Ahmad</v>
+        <v>Sameer Rizvi</v>
       </c>
       <c r="B126" t="str">
-        <v>GT</v>
+        <v>CSK</v>
       </c>
       <c r="C126" t="str">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>Devdutt Padikkal</v>
+        <v>Noor Ahmad</v>
       </c>
       <c r="B127" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C127" t="str">
         <v>7</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>Anukul Roy</v>
+        <v>Devdutt Padikkal</v>
       </c>
       <c r="B128" t="str">
-        <v>KKR</v>
+        <v>LSG</v>
       </c>
       <c r="C128" t="str">
         <v>7</v>
@@ -1790,87 +1790,87 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>David Miller</v>
+        <v>Anukul Roy</v>
       </c>
       <c r="B129" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C129" t="str">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>Rilee Rossouw</v>
+        <v>David Miller</v>
       </c>
       <c r="B130" t="str">
-        <v>PBKS</v>
+        <v>GT</v>
       </c>
       <c r="C130" t="str">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Glenn Maxwell</v>
+        <v>Rilee Rossouw</v>
       </c>
       <c r="B131" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C131" t="str">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>Romario Shepherd</v>
+        <v>Deepak Chahar</v>
       </c>
       <c r="B132" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C132" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>Marco Jansen</v>
+        <v>Matt Henry</v>
       </c>
       <c r="B133" t="str">
-        <v>SRH</v>
+        <v>LSG</v>
       </c>
       <c r="C133" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>Rahmanullah Gurbaz</v>
+        <v>Glenn Maxwell</v>
       </c>
       <c r="B134" t="str">
-        <v>KKR</v>
+        <v>RCB</v>
       </c>
       <c r="C134" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Wriddhiman Saha</v>
+        <v>Romario Shepherd</v>
       </c>
       <c r="B135" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C135" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>Kane Williamson</v>
+        <v>Marco Jansen</v>
       </c>
       <c r="B136" t="str">
-        <v>GT</v>
+        <v>SRH</v>
       </c>
       <c r="C136" t="str">
         <v>0</v>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Dilshan Madushanka</v>
+        <v>Wriddhiman Saha</v>
       </c>
       <c r="B137" t="str">
-        <v>MI</v>
+        <v>GT</v>
       </c>
       <c r="C137" t="str">
         <v>0</v>
@@ -1889,10 +1889,10 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Chris Woakes</v>
+        <v>Kane Williamson</v>
       </c>
       <c r="B138" t="str">
-        <v>PBKS</v>
+        <v>GT</v>
       </c>
       <c r="C138" t="str">
         <v>0</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Cameron Green</v>
+        <v>Chris Woakes</v>
       </c>
       <c r="B139" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C139" t="str">
         <v>0</v>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Mitchell Marsh</v>
+        <v>Dilshan Madushanka</v>
       </c>
       <c r="B140" t="str">
-        <v>DC</v>
+        <v>MI</v>
       </c>
       <c r="C140" t="str">
         <v>0</v>
@@ -1922,10 +1922,10 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>Mukesh Choudhary</v>
+        <v>Nathan Ellis</v>
       </c>
       <c r="B141" t="str">
-        <v>CSK</v>
+        <v>PBKS</v>
       </c>
       <c r="C141" t="str">
         <v>0</v>
@@ -1933,10 +1933,10 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>Nathan Ellis</v>
+        <v>Navdeep Saini</v>
       </c>
       <c r="B142" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C142" t="str">
         <v>0</v>
@@ -1944,10 +1944,10 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>Anrich Nortje</v>
+        <v>Mukesh Choudhary</v>
       </c>
       <c r="B143" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C143" t="str">
         <v>0</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>Deepak Chahar</v>
+        <v>Lalit Yadav</v>
       </c>
       <c r="B144" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C144" t="str">
         <v>0</v>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>Luke Wood</v>
+        <v>Alzarri Joseph</v>
       </c>
       <c r="B145" t="str">
-        <v>MI</v>
+        <v>RCB</v>
       </c>
       <c r="C145" t="str">
         <v>0</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>Lizaad Williams</v>
+        <v>Mitchell Marsh</v>
       </c>
       <c r="B146" t="str">
         <v>DC</v>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>Fazal Haque</v>
+        <v>Luke Wood</v>
       </c>
       <c r="B147" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C147" t="str">
         <v>0</v>
@@ -1999,10 +1999,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>Mitchell Santner</v>
+        <v>Lizaad Williams</v>
       </c>
       <c r="B148" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C148" t="str">
         <v>0</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Krishnappa Gowtham</v>
+        <v>Fazal Haque</v>
       </c>
       <c r="B149" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C149" t="str">
         <v>0</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>Kyle Mayers</v>
+        <v>Mitchell Santner</v>
       </c>
       <c r="B150" t="str">
-        <v>LSG</v>
+        <v>CSK</v>
       </c>
       <c r="C150" t="str">
         <v>0</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>Kumar Kushagra</v>
+        <v>Krishnappa Gowtham</v>
       </c>
       <c r="B151" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C151" t="str">
         <v>0</v>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>Nehal Wadhera</v>
+        <v>Kyle Mayers</v>
       </c>
       <c r="B152" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C152" t="str">
         <v>0</v>
@@ -2054,10 +2054,10 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>Amit Mishra</v>
+        <v>Nehal Wadhera</v>
       </c>
       <c r="B153" t="str">
-        <v>LSG</v>
+        <v>MI</v>
       </c>
       <c r="C153" t="str">
         <v>0</v>
@@ -2065,10 +2065,10 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Moeen Ali</v>
+        <v>Kumar Kushagra</v>
       </c>
       <c r="B154" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C154" t="str">
         <v>0</v>
@@ -2076,10 +2076,10 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>Suyash Prabhudessai</v>
+        <v>Amit Mishra</v>
       </c>
       <c r="B155" t="str">
-        <v>RCB</v>
+        <v>LSG</v>
       </c>
       <c r="C155" t="str">
         <v>0</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Washington Sundar</v>
+        <v>Suyash Prabhudessai</v>
       </c>
       <c r="B157" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C157" t="str">
         <v>0</v>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>Suyash Sharma</v>
+        <v>Washington Sundar</v>
       </c>
       <c r="B158" t="str">
-        <v>KKR</v>
+        <v>SRH</v>
       </c>
       <c r="C158" t="str">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>Manish Pandey</v>
+        <v>Anrich Nortje</v>
       </c>
       <c r="B159" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C159" t="str">
         <v>0</v>
@@ -2131,10 +2131,10 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>Karn Sharma</v>
+        <v>Manish Pandey</v>
       </c>
       <c r="B160" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C160" t="str">
         <v>0</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>Sandeep Sharma</v>
+        <v>Karn Sharma</v>
       </c>
       <c r="B161" t="str">
-        <v>RR</v>
+        <v>RCB</v>
       </c>
       <c r="C161" t="str">
         <v>0</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>Yash Dhull</v>
+        <v>Sandeep Sharma</v>
       </c>
       <c r="B162" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C162" t="str">
         <v>0</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>Umran Malik</v>
+        <v>Yash Dhull</v>
       </c>
       <c r="B163" t="str">
-        <v>SRH</v>
+        <v>DC</v>
       </c>
       <c r="C163" t="str">
         <v>0</v>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>Nitish Rana</v>
+        <v>Umran Malik</v>
       </c>
       <c r="B164" t="str">
-        <v>KKR</v>
+        <v>SRH</v>
       </c>
       <c r="C164" t="str">
         <v>0</v>
@@ -2186,10 +2186,10 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>Azmatullah Omarzai</v>
+        <v>Nitish Rana</v>
       </c>
       <c r="B165" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C165" t="str">
         <v>0</v>
@@ -2197,10 +2197,10 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>Rahul Chahar</v>
+        <v>Azmatullah Omarzai</v>
       </c>
       <c r="B166" t="str">
-        <v>PBKS</v>
+        <v>GT</v>
       </c>
       <c r="C166" t="str">
         <v>0</v>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>Kwena Maphaka</v>
+        <v>Rahul Chahar</v>
       </c>
       <c r="B167" t="str">
-        <v>MI</v>
+        <v>PBKS</v>
       </c>
       <c r="C167" t="str">
         <v>0</v>
@@ -2219,10 +2219,10 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>Keshav Maharaj</v>
+        <v>Kwena Maphaka</v>
       </c>
       <c r="B168" t="str">
-        <v>RR</v>
+        <v>MI</v>
       </c>
       <c r="C168" t="str">
         <v>0</v>
@@ -2230,10 +2230,10 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Dushmantha Chameera</v>
+        <v>Keshav Maharaj</v>
       </c>
       <c r="B169" t="str">
-        <v>KKR</v>
+        <v>RR</v>
       </c>
       <c r="C169" t="str">
         <v>0</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Manav Suthar</v>
+        <v>Dushmantha Chameera</v>
       </c>
       <c r="B170" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C170" t="str">
         <v>0</v>
@@ -2252,10 +2252,10 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Praveen Dubey</v>
+        <v>Manav Suthar</v>
       </c>
       <c r="B171" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C171" t="str">
         <v>0</v>
@@ -2263,10 +2263,10 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Simarjeet Singh</v>
+        <v>Praveen Dubey</v>
       </c>
       <c r="B172" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C172" t="str">
         <v>0</v>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Jhye Richardson</v>
+        <v>Cameron Green</v>
       </c>
       <c r="B174" t="str">
-        <v>DC</v>
+        <v>RCB</v>
       </c>
       <c r="C174" t="str">
         <v>0</v>
@@ -2296,10 +2296,10 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Rishi Dhawan</v>
+        <v>Rahmanullah Gurbaz</v>
       </c>
       <c r="B175" t="str">
-        <v>PBKS</v>
+        <v>KKR</v>
       </c>
       <c r="C175" t="str">
         <v>0</v>
@@ -2307,10 +2307,10 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Shamar Joseph</v>
+        <v>Suyash Sharma</v>
       </c>
       <c r="B176" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C176" t="str">
         <v>0</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Jason Behrendorff</v>
+        <v>Jhye Richardson</v>
       </c>
       <c r="B177" t="str">
-        <v>MI</v>
+        <v>DC</v>
       </c>
       <c r="C177" t="str">
         <v>0</v>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Navdeep Saini</v>
+        <v>Rishi Dhawan</v>
       </c>
       <c r="B178" t="str">
-        <v>RR</v>
+        <v>PBKS</v>
       </c>
       <c r="C178" t="str">
         <v>0</v>
@@ -2340,10 +2340,10 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>Alzarri Joseph</v>
+        <v>Dewald Brevis</v>
       </c>
       <c r="B179" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C179" t="str">
         <v>0</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Lalit Yadav</v>
+        <v>Simarjeet Singh</v>
       </c>
       <c r="B180" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C180" t="str">
         <v>0</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Dewald Brevis</v>
+        <v>Jason Behrendorff</v>
       </c>
       <c r="B181" t="str">
         <v>MI</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Tom Kohler-Cadmore</v>
+        <v>Donavon Ferreira</v>
       </c>
       <c r="B182" t="str">
         <v>RR</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>SK Rasheed</v>
+        <v>Sherfane Rutherford</v>
       </c>
       <c r="B183" t="str">
-        <v>CSK</v>
+        <v>KKR</v>
       </c>
       <c r="C183" t="str">
         <v>0</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Donavon Ferreira</v>
+        <v>Tom Kohler-Cadmore</v>
       </c>
       <c r="B184" t="str">
         <v>RR</v>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>Kunal Singh Rathore</v>
+        <v>Shamar Joseph</v>
       </c>
       <c r="B185" t="str">
-        <v>RR</v>
+        <v>LSG</v>
       </c>
       <c r="C185" t="str">
         <v>0</v>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>M Siddharth</v>
+        <v>Glenn Phillips</v>
       </c>
       <c r="B186" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C186" t="str">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Sherfane Rutherford</v>
+        <v>Kunal Singh Rathore</v>
       </c>
       <c r="B187" t="str">
-        <v>KKR</v>
+        <v>RR</v>
       </c>
       <c r="C187" t="str">
         <v>0</v>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Glenn Phillips</v>
+        <v>Mayank Dagar</v>
       </c>
       <c r="B189" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C189" t="str">
         <v>0</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Piyush Chawla</v>
+        <v>Mayank Agarwal</v>
       </c>
       <c r="B190" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C190" t="str">
         <v>0</v>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>Matt Henry</v>
+        <v>M Siddharth</v>
       </c>
       <c r="B191" t="str">
         <v>LSG</v>
@@ -2483,10 +2483,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>Mayank Dagar</v>
+        <v>SK Rasheed</v>
       </c>
       <c r="B192" t="str">
-        <v>RCB</v>
+        <v>CSK</v>
       </c>
       <c r="C192" t="str">
         <v>0</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Mayank Agarwal</v>
+        <v>Piyush Chawla</v>
       </c>
       <c r="B193" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C193" t="str">
         <v>0</v>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>BR sharath</v>
+        <v>Allah Ghazanfar</v>
       </c>
       <c r="B194" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C194" t="str">
         <v>0</v>
@@ -2527,10 +2527,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Allah Ghazanfar</v>
+        <v>Sandeep Warrier</v>
       </c>
       <c r="B196" t="str">
-        <v>KKR</v>
+        <v>GT</v>
       </c>
       <c r="C196" t="str">
         <v>0</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Sandeep Warrier</v>
+        <v>BR sharath</v>
       </c>
       <c r="B197" t="str">
         <v>GT</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Ajay Mandal</v>
+        <v>Tanay Thyagarajan</v>
       </c>
       <c r="B198" t="str">
-        <v>CSK</v>
+        <v>PBKS</v>
       </c>
       <c r="C198" t="str">
         <v>0</v>
@@ -2560,10 +2560,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Ashton Turner</v>
+        <v>Anshul Kamboj</v>
       </c>
       <c r="B199" t="str">
-        <v>LSG</v>
+        <v>MI</v>
       </c>
       <c r="C199" t="str">
         <v>0</v>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Tanay Thyagarajan</v>
+        <v>Ajay Mandal</v>
       </c>
       <c r="B200" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C200" t="str">
         <v>0</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Anshul Kamboj</v>
+        <v>Shivalik Sharma</v>
       </c>
       <c r="B201" t="str">
         <v>MI</v>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Nishant Sindhu</v>
+        <v>Ashton Turner</v>
       </c>
       <c r="B202" t="str">
-        <v>CSK</v>
+        <v>LSG</v>
       </c>
       <c r="C202" t="str">
         <v>0</v>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Yudhvir Singh</v>
+        <v>Nishant Sindhu</v>
       </c>
       <c r="B203" t="str">
-        <v>LSG</v>
+        <v>CSK</v>
       </c>
       <c r="C203" t="str">
         <v>0</v>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Shivalik Sharma</v>
+        <v>Prerak Mankad</v>
       </c>
       <c r="B204" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C204" t="str">
         <v>0</v>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Shams Mulani</v>
+        <v>Yudhvir Singh</v>
       </c>
       <c r="B205" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C205" t="str">
         <v>0</v>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Jhatavedh Subramanyan</v>
+        <v>Shams Mulani</v>
       </c>
       <c r="B206" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C206" t="str">
         <v>0</v>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Sanvir Singh</v>
+        <v>Arshin Kulkarni</v>
       </c>
       <c r="B207" t="str">
-        <v>SRH</v>
+        <v>LSG</v>
       </c>
       <c r="C207" t="str">
         <v>0</v>
@@ -2659,10 +2659,10 @@
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>Rasikh Dar</v>
+        <v>Jhatavedh Subramanyan</v>
       </c>
       <c r="B208" t="str">
-        <v>DC</v>
+        <v>SRH</v>
       </c>
       <c r="C208" t="str">
         <v>0</v>
@@ -2692,10 +2692,10 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>Prashant Solanki</v>
+        <v>Sanvir Singh</v>
       </c>
       <c r="B211" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C211" t="str">
         <v>0</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>Joshua Little</v>
+        <v>Rasikh Dar</v>
       </c>
       <c r="B213" t="str">
-        <v>GT</v>
+        <v>DC</v>
       </c>
       <c r="C213" t="str">
         <v>0</v>
@@ -2725,10 +2725,10 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Vishwapratap Singh</v>
+        <v>Prashant Solanki</v>
       </c>
       <c r="B214" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C214" t="str">
         <v>0</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>Jayant Yadav</v>
+        <v>Vishwapratap Singh</v>
       </c>
       <c r="B215" t="str">
-        <v>GT</v>
+        <v>PBKS</v>
       </c>
       <c r="C215" t="str">
         <v>0</v>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Sushant Mishra</v>
+        <v>Joshua Little</v>
       </c>
       <c r="B216" t="str">
         <v>GT</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Kartik Tyagi</v>
+        <v>Jayant Yadav</v>
       </c>
       <c r="B217" t="str">
         <v>GT</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>Prerak Mankad</v>
+        <v>Sushant Mishra</v>
       </c>
       <c r="B218" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C218" t="str">
         <v>0</v>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="220">
       <c r="A220" t="str">
-        <v>Arshin Kulkarni</v>
+        <v>Sakib Hussain</v>
       </c>
       <c r="B220" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C220" t="str">
         <v>0</v>
@@ -2802,10 +2802,10 @@
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>Sakib Hussain</v>
+        <v>Kartik Tyagi</v>
       </c>
       <c r="B221" t="str">
-        <v>KKR</v>
+        <v>GT</v>
       </c>
       <c r="C221" t="str">
         <v>0</v>
@@ -2813,10 +2813,10 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>Tom Curran</v>
+        <v>Vidhwath Kaverappa</v>
       </c>
       <c r="B222" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C222" t="str">
         <v>0</v>
@@ -2824,10 +2824,10 @@
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>Rajvardhan Hangargekar</v>
+        <v>Tom Curran</v>
       </c>
       <c r="B223" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C223" t="str">
         <v>0</v>
@@ -2846,10 +2846,10 @@
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>Vidhwath Kaverappa</v>
+        <v>Abid Mushtaq</v>
       </c>
       <c r="B225" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C225" t="str">
         <v>0</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>Ricky Bhui</v>
+        <v>Rajvardhan Hangargekar</v>
       </c>
       <c r="B227" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C227" t="str">
         <v>0</v>
@@ -2890,10 +2890,10 @@
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>Aravelly Avanish</v>
+        <v>Himanshu Sharma</v>
       </c>
       <c r="B229" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C229" t="str">
         <v>0</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>Nuwan Thushara</v>
+        <v>Aravelly Avanish</v>
       </c>
       <c r="B230" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C230" t="str">
         <v>0</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>Himanshu Sharma</v>
+        <v>Shivam Singh</v>
       </c>
       <c r="B231" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C231" t="str">
         <v>0</v>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>Shivam Singh</v>
+        <v>Anmolpreet Singh</v>
       </c>
       <c r="B232" t="str">
-        <v>PBKS</v>
+        <v>SRH</v>
       </c>
       <c r="C232" t="str">
         <v>0</v>
@@ -2934,10 +2934,10 @@
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>Naman Dhir</v>
+        <v>Upendra Yadav</v>
       </c>
       <c r="B233" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C233" t="str">
         <v>0</v>
@@ -2945,10 +2945,10 @@
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>Abid Mushtaq</v>
+        <v>Ricky Bhui</v>
       </c>
       <c r="B234" t="str">
-        <v>RR</v>
+        <v>DC</v>
       </c>
       <c r="C234" t="str">
         <v>0</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>Upendra Yadav</v>
+        <v>Kumar Kartikeya</v>
       </c>
       <c r="B235" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C235" t="str">
         <v>0</v>
@@ -2967,10 +2967,10 @@
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>Darshan Nalkande</v>
+        <v>Nuwan Thushara</v>
       </c>
       <c r="B236" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C236" t="str">
         <v>0</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>Vishnu Vinod</v>
+        <v>Naman Dhir</v>
       </c>
       <c r="B237" t="str">
         <v>MI</v>
@@ -2989,10 +2989,10 @@
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>Kumar Kartikeya</v>
+        <v>Darshan Nalkande</v>
       </c>
       <c r="B238" t="str">
-        <v>MI</v>
+        <v>GT</v>
       </c>
       <c r="C238" t="str">
         <v>0</v>
@@ -3000,10 +3000,10 @@
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>Anmolpreet Singh</v>
+        <v>Vishnu Vinod</v>
       </c>
       <c r="B239" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C239" t="str">
         <v>0</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>Mohammed Siraj</v>
+        <v>Yash Dayal</v>
       </c>
       <c r="B244" t="str">
         <v>RCB</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>Yash Dayal</v>
+        <v>Mohammed Siraj</v>
       </c>
       <c r="B245" t="str">
         <v>RCB</v>

</xml_diff>

<commit_message>
20/4 Srh vs Dc
</commit_message>
<xml_diff>
--- a/frontend/public/Apr16.xlsx
+++ b/frontend/public/Apr16.xlsx
@@ -404,343 +404,343 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>KL Rahul</v>
+        <v>Travis Head</v>
       </c>
       <c r="B3" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C3" t="str">
-        <v>277</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Rohit Sharma</v>
+        <v>KL Rahul</v>
       </c>
       <c r="B4" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C4" t="str">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Jasprit Bumrah</v>
+        <v>Rohit Sharma</v>
       </c>
       <c r="B5" t="str">
         <v>MI</v>
       </c>
       <c r="C5" t="str">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Sam Curran</v>
+        <v>Jasprit Bumrah</v>
       </c>
       <c r="B6" t="str">
-        <v>PBKS</v>
+        <v>MI</v>
       </c>
       <c r="C6" t="str">
-        <v>224</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Ruturaj Gaikwad</v>
+        <v>Nithish Reddy</v>
       </c>
       <c r="B7" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C7" t="str">
-        <v>214</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Ashutosh Sharma</v>
+        <v>Sam Curran</v>
       </c>
       <c r="B8" t="str">
         <v>PBKS</v>
       </c>
       <c r="C8" t="str">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Ishan Kishan</v>
+        <v>T Natarajan</v>
       </c>
       <c r="B9" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C9" t="str">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Dinesh Karthik</v>
+        <v>Ruturaj Gaikwad</v>
       </c>
       <c r="B10" t="str">
-        <v>RCB</v>
+        <v>CSK</v>
       </c>
       <c r="C10" t="str">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Ravindra Jadeja</v>
+        <v>Kuldeep Yadav</v>
       </c>
       <c r="B11" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C11" t="str">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Riyan Parag</v>
+        <v>Ravindra Jadeja</v>
       </c>
       <c r="B12" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C12" t="str">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Kuldeep Sen</v>
+        <v>Dinesh Karthik</v>
       </c>
       <c r="B13" t="str">
-        <v>RR</v>
+        <v>RCB</v>
       </c>
       <c r="C13" t="str">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Suryakumar Yadav</v>
+        <v>Rishabh Pant</v>
       </c>
       <c r="B14" t="str">
-        <v>MI</v>
+        <v>DC</v>
       </c>
       <c r="C14" t="str">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Faf du Plessis</v>
+        <v>Ashutosh Sharma</v>
       </c>
       <c r="B15" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C15" t="str">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Harshal Patel</v>
+        <v>Ishan Kishan</v>
       </c>
       <c r="B16" t="str">
-        <v>PBKS</v>
+        <v>MI</v>
       </c>
       <c r="C16" t="str">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Shashank Singh</v>
+        <v>Riyan Parag</v>
       </c>
       <c r="B17" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C17" t="str">
-        <v>167</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Travis Head</v>
+        <v>Harshal Patel</v>
       </c>
       <c r="B18" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C18" t="str">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Jos Buttler</v>
+        <v>Kuldeep Sen</v>
       </c>
       <c r="B19" t="str">
         <v>RR</v>
       </c>
       <c r="C19" t="str">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Philip Salt</v>
+        <v>Heinrich Klaasen</v>
       </c>
       <c r="B20" t="str">
-        <v>KKR</v>
+        <v>SRH</v>
       </c>
       <c r="C20" t="str">
-        <v>160</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Sanju Samson</v>
+        <v>Suryakumar Yadav</v>
       </c>
       <c r="B21" t="str">
-        <v>RR</v>
+        <v>MI</v>
       </c>
       <c r="C21" t="str">
-        <v>158</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Kagiso Rabada</v>
+        <v>Faf du Plessis</v>
       </c>
       <c r="B22" t="str">
-        <v>PBKS</v>
+        <v>RCB</v>
       </c>
       <c r="C22" t="str">
-        <v>158</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Avesh Khan</v>
+        <v>Jos Buttler</v>
       </c>
       <c r="B23" t="str">
         <v>RR</v>
       </c>
       <c r="C23" t="str">
-        <v>153</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Heinrich Klaasen</v>
+        <v>Shashank Singh</v>
       </c>
       <c r="B24" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C24" t="str">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Matheesha Pathirana</v>
+        <v>Pat Cummins</v>
       </c>
       <c r="B25" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C25" t="str">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Pat Cummins</v>
+        <v>Abhishek Sharma</v>
       </c>
       <c r="B26" t="str">
         <v>SRH</v>
       </c>
       <c r="C26" t="str">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Arshdeep Singh</v>
+        <v>Philip Salt</v>
       </c>
       <c r="B27" t="str">
-        <v>PBKS</v>
+        <v>KKR</v>
       </c>
       <c r="C27" t="str">
-        <v>137</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Gerald Coetzee</v>
+        <v>Kagiso Rabada</v>
       </c>
       <c r="B28" t="str">
-        <v>MI</v>
+        <v>PBKS</v>
       </c>
       <c r="C28" t="str">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Rishabh Pant</v>
+        <v>Sanju Samson</v>
       </c>
       <c r="B29" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C29" t="str">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Shivam Dube</v>
+        <v>Matheesha Pathirana</v>
       </c>
       <c r="B30" t="str">
         <v>CSK</v>
       </c>
       <c r="C30" t="str">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Tilak Varma</v>
+        <v>Avesh Khan</v>
       </c>
       <c r="B31" t="str">
-        <v>MI</v>
+        <v>RR</v>
       </c>
       <c r="C31" t="str">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Rashid Khan</v>
+        <v>Gerald Coetzee</v>
       </c>
       <c r="B32" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C32" t="str">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Hardik Pandya</v>
+        <v>Shivam Dube</v>
       </c>
       <c r="B33" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C33" t="str">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34">
@@ -751,546 +751,546 @@
         <v>DC</v>
       </c>
       <c r="C34" t="str">
-        <v>130</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Shreyas Iyer</v>
+        <v>Jack Fraser-Mcgurk</v>
       </c>
       <c r="B35" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C35" t="str">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Ayush Badoni</v>
+        <v>Arshdeep Singh</v>
       </c>
       <c r="B36" t="str">
-        <v>LSG</v>
+        <v>PBKS</v>
       </c>
       <c r="C36" t="str">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Tushar Deshpande</v>
+        <v>Tilak Varma</v>
       </c>
       <c r="B37" t="str">
-        <v>CSK</v>
+        <v>MI</v>
       </c>
       <c r="C37" t="str">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Yuzvendra Chahal</v>
+        <v>Rashid Khan</v>
       </c>
       <c r="B38" t="str">
-        <v>RR</v>
+        <v>GT</v>
       </c>
       <c r="C38" t="str">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Quinton de Kock</v>
+        <v>Hardik Pandya</v>
       </c>
       <c r="B39" t="str">
-        <v>LSG</v>
+        <v>MI</v>
       </c>
       <c r="C39" t="str">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Mustafizur Rahman</v>
+        <v>Abdul Samad</v>
       </c>
       <c r="B40" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C40" t="str">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Khaleel Ahmed</v>
+        <v>Ayush Badoni</v>
       </c>
       <c r="B41" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C41" t="str">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Yashasvi Jaiswal</v>
+        <v>Shreyas Iyer</v>
       </c>
       <c r="B42" t="str">
-        <v>RR</v>
+        <v>KKR</v>
       </c>
       <c r="C42" t="str">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Nicholas Pooran</v>
+        <v>Tushar Deshpande</v>
       </c>
       <c r="B43" t="str">
-        <v>LSG</v>
+        <v>CSK</v>
       </c>
       <c r="C43" t="str">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Shubman Gill</v>
+        <v>Shahbaz Ahmed</v>
       </c>
       <c r="B44" t="str">
-        <v>GT</v>
+        <v>SRH</v>
       </c>
       <c r="C44" t="str">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Vaibhav Arora</v>
+        <v>Yuzvendra Chahal</v>
       </c>
       <c r="B45" t="str">
-        <v>KKR</v>
+        <v>RR</v>
       </c>
       <c r="C45" t="str">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Nithish Reddy</v>
+        <v>Quinton de Kock</v>
       </c>
       <c r="B46" t="str">
-        <v>SRH</v>
+        <v>LSG</v>
       </c>
       <c r="C46" t="str">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Jitesh Sharma</v>
+        <v>Mustafizur Rahman</v>
       </c>
       <c r="B47" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C47" t="str">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Kuldeep Yadav</v>
+        <v>Yashasvi Jaiswal</v>
       </c>
       <c r="B48" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C48" t="str">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Abdul Samad</v>
+        <v>Nicholas Pooran</v>
       </c>
       <c r="B49" t="str">
-        <v>SRH</v>
+        <v>LSG</v>
       </c>
       <c r="C49" t="str">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Mitchell Starc</v>
+        <v>Khaleel Ahmed</v>
       </c>
       <c r="B50" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C50" t="str">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Varun Chakravarthy</v>
+        <v>Vaibhav Arora</v>
       </c>
       <c r="B51" t="str">
         <v>KKR</v>
       </c>
       <c r="C51" t="str">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Shreyas Gopal</v>
+        <v>Angkrish Raghuvanshi</v>
       </c>
       <c r="B52" t="str">
-        <v>MI</v>
+        <v>KKR</v>
       </c>
       <c r="C52" t="str">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Angkrish Raghuvanshi</v>
+        <v>Axar Patel</v>
       </c>
       <c r="B53" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C53" t="str">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Ishant Sharma</v>
+        <v>Shubman Gill</v>
       </c>
       <c r="B54" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C54" t="str">
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Rajat Patidar</v>
+        <v>Jitesh Sharma</v>
       </c>
       <c r="B55" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C55" t="str">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>Mohsin Khan</v>
+        <v>Mayank Markande</v>
       </c>
       <c r="B56" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C56" t="str">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Ravi Bishnoi</v>
+        <v>Tristan Stubbs</v>
       </c>
       <c r="B57" t="str">
-        <v>LSG</v>
+        <v>DC</v>
       </c>
       <c r="C57" t="str">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Virat Kohli</v>
+        <v>Mitchell Starc</v>
       </c>
       <c r="B58" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C58" t="str">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Marcus Stoinis</v>
+        <v>Bhuvneshwar Kumar</v>
       </c>
       <c r="B59" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C59" t="str">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Liam Livingstone</v>
+        <v>Varun Chakravarthy</v>
       </c>
       <c r="B60" t="str">
-        <v>PBKS</v>
+        <v>KKR</v>
       </c>
       <c r="C60" t="str">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Abhishek Sharma</v>
+        <v>Shreyas Gopal</v>
       </c>
       <c r="B61" t="str">
-        <v>SRH</v>
+        <v>MI</v>
       </c>
       <c r="C61" t="str">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Trent Boult</v>
+        <v>Ishant Sharma</v>
       </c>
       <c r="B62" t="str">
-        <v>RR</v>
+        <v>DC</v>
       </c>
       <c r="C62" t="str">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>MS Dhoni</v>
+        <v>Prithvi Shaw</v>
       </c>
       <c r="B63" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C63" t="str">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Krunal Pandya</v>
+        <v>Rajat Patidar</v>
       </c>
       <c r="B64" t="str">
-        <v>LSG</v>
+        <v>RCB</v>
       </c>
       <c r="C64" t="str">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Tristan Stubbs</v>
+        <v>Abhishek Porel</v>
       </c>
       <c r="B65" t="str">
         <v>DC</v>
       </c>
       <c r="C65" t="str">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Andre Russell</v>
+        <v>Ravi Bishnoi</v>
       </c>
       <c r="B66" t="str">
-        <v>KKR</v>
+        <v>LSG</v>
       </c>
       <c r="C66" t="str">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Shimron Hetmyer</v>
+        <v>Virat Kohli</v>
       </c>
       <c r="B67" t="str">
-        <v>RR</v>
+        <v>RCB</v>
       </c>
       <c r="C67" t="str">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Daryl Mitchell</v>
+        <v>Marcus Stoinis</v>
       </c>
       <c r="B68" t="str">
-        <v>CSK</v>
+        <v>LSG</v>
       </c>
       <c r="C68" t="str">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Rachin Ravindra</v>
+        <v>Trent Boult</v>
       </c>
       <c r="B69" t="str">
-        <v>CSK</v>
+        <v>RR</v>
       </c>
       <c r="C69" t="str">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Bhuvneshwar Kumar</v>
+        <v>Liam Livingstone</v>
       </c>
       <c r="B70" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C70" t="str">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Ajinkya Rahane</v>
+        <v>Mohsin Khan</v>
       </c>
       <c r="B71" t="str">
-        <v>CSK</v>
+        <v>LSG</v>
       </c>
       <c r="C71" t="str">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Prithvi Shaw</v>
+        <v>Shimron Hetmyer</v>
       </c>
       <c r="B72" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C72" t="str">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>B Sai Sudharsan</v>
+        <v>Krunal Pandya</v>
       </c>
       <c r="B73" t="str">
-        <v>GT</v>
+        <v>LSG</v>
       </c>
       <c r="C73" t="str">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Tim David</v>
+        <v>Andre Russell</v>
       </c>
       <c r="B74" t="str">
-        <v>MI</v>
+        <v>KKR</v>
       </c>
       <c r="C74" t="str">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Harpreet Brar</v>
+        <v>Rachin Ravindra</v>
       </c>
       <c r="B75" t="str">
-        <v>PBKS</v>
+        <v>CSK</v>
       </c>
       <c r="C75" t="str">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Mohammad Nabi</v>
+        <v>Ajinkya Rahane</v>
       </c>
       <c r="B76" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C76" t="str">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Rovman Powell</v>
+        <v>Daryl Mitchell</v>
       </c>
       <c r="B77" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C77" t="str">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>Dhruv Jurel</v>
+        <v>MS Dhoni</v>
       </c>
       <c r="B78" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C78" t="str">
-        <v>60</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>Akash Madhwal</v>
+        <v>Harpreet Brar</v>
       </c>
       <c r="B79" t="str">
-        <v>MI</v>
+        <v>PBKS</v>
       </c>
       <c r="C79" t="str">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>Yash Thakur</v>
+        <v>Mohammad Nabi</v>
       </c>
       <c r="B80" t="str">
-        <v>LSG</v>
+        <v>MI</v>
       </c>
       <c r="C80" t="str">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>Mayank Markande</v>
+        <v>Rovman Powell</v>
       </c>
       <c r="B81" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C81" t="str">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>Rahul Tewatia</v>
+        <v>Akash Madhwal</v>
       </c>
       <c r="B82" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C82" t="str">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>Lockie Ferguson</v>
+        <v>Yash Thakur</v>
       </c>
       <c r="B83" t="str">
-        <v>RCB</v>
+        <v>LSG</v>
       </c>
       <c r="C83" t="str">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84">
@@ -1301,89 +1301,89 @@
         <v>SRH</v>
       </c>
       <c r="C84" t="str">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>Harshit Rana</v>
+        <v>Rahul Tewatia</v>
       </c>
       <c r="B85" t="str">
-        <v>KKR</v>
+        <v>GT</v>
       </c>
       <c r="C85" t="str">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>T Natarajan</v>
+        <v>B Sai Sudharsan</v>
       </c>
       <c r="B86" t="str">
-        <v>SRH</v>
+        <v>GT</v>
       </c>
       <c r="C86" t="str">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>Shai Hope</v>
+        <v>Tim David</v>
       </c>
       <c r="B87" t="str">
-        <v>DC</v>
+        <v>MI</v>
       </c>
       <c r="C87" t="str">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>Axar Patel</v>
+        <v>Dhruv Jurel</v>
       </c>
       <c r="B88" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C88" t="str">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>Moeen Ali</v>
+        <v>Shai Hope</v>
       </c>
       <c r="B89" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C89" t="str">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>Maheesh Theekshana</v>
+        <v>Moeen Ali</v>
       </c>
       <c r="B90" t="str">
         <v>CSK</v>
       </c>
       <c r="C90" t="str">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>Rinku Singh</v>
+        <v>Maheesh Theekshana</v>
       </c>
       <c r="B91" t="str">
-        <v>KKR</v>
+        <v>CSK</v>
       </c>
       <c r="C91" t="str">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>Ramandeep Singh</v>
+        <v>Rinku Singh</v>
       </c>
       <c r="B92" t="str">
         <v>KKR</v>
@@ -1394,18 +1394,18 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Mahipal Lomror</v>
+        <v>Ramandeep Singh</v>
       </c>
       <c r="B93" t="str">
-        <v>RCB</v>
+        <v>KKR</v>
       </c>
       <c r="C93" t="str">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>Will Jacks</v>
+        <v>Mahipal Lomror</v>
       </c>
       <c r="B94" t="str">
         <v>RCB</v>
@@ -1416,24 +1416,24 @@
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>Jaydev Unadkat</v>
+        <v>Harshit Rana</v>
       </c>
       <c r="B95" t="str">
-        <v>SRH</v>
+        <v>KKR</v>
       </c>
       <c r="C95" t="str">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>Anuj Rawat</v>
+        <v>Lockie Ferguson</v>
       </c>
       <c r="B96" t="str">
         <v>RCB</v>
       </c>
       <c r="C96" t="str">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97">
@@ -1449,35 +1449,35 @@
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>Spencer Johnson</v>
+        <v>Anuj Rawat</v>
       </c>
       <c r="B98" t="str">
-        <v>GT</v>
+        <v>RCB</v>
       </c>
       <c r="C98" t="str">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>Mohit Sharma</v>
+        <v>Spencer Johnson</v>
       </c>
       <c r="B99" t="str">
         <v>GT</v>
       </c>
       <c r="C99" t="str">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>Jack Fraser-Mcgurk</v>
+        <v>Mohit Sharma</v>
       </c>
       <c r="B100" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C100" t="str">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101">
@@ -1515,21 +1515,21 @@
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>Simran Singh</v>
+        <v>Jaydev Unadkat</v>
       </c>
       <c r="B104" t="str">
-        <v>PBKS</v>
+        <v>SRH</v>
       </c>
       <c r="C104" t="str">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Vyshak Vijay Kumar</v>
+        <v>Simran Singh</v>
       </c>
       <c r="B105" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C105" t="str">
         <v>34</v>
@@ -1537,32 +1537,32 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>Venkatesh Iyer</v>
+        <v>Vyshak Vijay Kumar</v>
       </c>
       <c r="B106" t="str">
-        <v>KKR</v>
+        <v>RCB</v>
       </c>
       <c r="C106" t="str">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Deepak Hooda</v>
+        <v>Venkatesh Iyer</v>
       </c>
       <c r="B107" t="str">
-        <v>LSG</v>
+        <v>KKR</v>
       </c>
       <c r="C107" t="str">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Reece Topley</v>
+        <v>Deepak Hooda</v>
       </c>
       <c r="B108" t="str">
-        <v>RCB</v>
+        <v>LSG</v>
       </c>
       <c r="C108" t="str">
         <v>31</v>
@@ -1570,46 +1570,46 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Jonny Bairstow</v>
+        <v>Will Jacks</v>
       </c>
       <c r="B109" t="str">
-        <v>PBKS</v>
+        <v>RCB</v>
       </c>
       <c r="C109" t="str">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Naveen-ul-Haq</v>
+        <v>Jonny Bairstow</v>
       </c>
       <c r="B110" t="str">
-        <v>LSG</v>
+        <v>PBKS</v>
       </c>
       <c r="C110" t="str">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Shikhar Dhawan</v>
+        <v>Naveen-ul-Haq</v>
       </c>
       <c r="B111" t="str">
-        <v>PBKS</v>
+        <v>LSG</v>
       </c>
       <c r="C111" t="str">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Abhishek Porel</v>
+        <v>Shikhar Dhawan</v>
       </c>
       <c r="B112" t="str">
-        <v>DC</v>
+        <v>PBKS</v>
       </c>
       <c r="C112" t="str">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113">
@@ -1636,24 +1636,24 @@
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>Shahbaz Ahmed</v>
+        <v>Shardul Thakur</v>
       </c>
       <c r="B115" t="str">
-        <v>SRH</v>
+        <v>CSK</v>
       </c>
       <c r="C115" t="str">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>Shardul Thakur</v>
+        <v>Washington Sundar</v>
       </c>
       <c r="B116" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C116" t="str">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117">
@@ -1686,18 +1686,18 @@
         <v>DC</v>
       </c>
       <c r="C119" t="str">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Harpreet Singh</v>
+        <v>Reece Topley</v>
       </c>
       <c r="B120" t="str">
-        <v>PBKS</v>
+        <v>RCB</v>
       </c>
       <c r="C120" t="str">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121">
@@ -1713,32 +1713,32 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>Ravichandran Ashwin</v>
+        <v>Harpreet Singh</v>
       </c>
       <c r="B122" t="str">
-        <v>RR</v>
+        <v>PBKS</v>
       </c>
       <c r="C122" t="str">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>Rahul Tripathi</v>
+        <v>Ravichandran Ashwin</v>
       </c>
       <c r="B123" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C123" t="str">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>Matthew Wade</v>
+        <v>Rahul Tripathi</v>
       </c>
       <c r="B124" t="str">
-        <v>GT</v>
+        <v>SRH</v>
       </c>
       <c r="C124" t="str">
         <v>16</v>
@@ -1768,21 +1768,21 @@
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>Noor Ahmad</v>
+        <v>Anrich Nortje</v>
       </c>
       <c r="B127" t="str">
-        <v>GT</v>
+        <v>DC</v>
       </c>
       <c r="C127" t="str">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>Devdutt Padikkal</v>
+        <v>Noor Ahmad</v>
       </c>
       <c r="B128" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C128" t="str">
         <v>7</v>
@@ -1790,10 +1790,10 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>Anukul Roy</v>
+        <v>Devdutt Padikkal</v>
       </c>
       <c r="B129" t="str">
-        <v>KKR</v>
+        <v>LSG</v>
       </c>
       <c r="C129" t="str">
         <v>7</v>
@@ -1801,98 +1801,98 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>David Miller</v>
+        <v>Anukul Roy</v>
       </c>
       <c r="B130" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C130" t="str">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Rilee Rossouw</v>
+        <v>David Miller</v>
       </c>
       <c r="B131" t="str">
-        <v>PBKS</v>
+        <v>GT</v>
       </c>
       <c r="C131" t="str">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>Deepak Chahar</v>
+        <v>Lalit Yadav</v>
       </c>
       <c r="B132" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C132" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>Matt Henry</v>
+        <v>Rilee Rossouw</v>
       </c>
       <c r="B133" t="str">
-        <v>LSG</v>
+        <v>PBKS</v>
       </c>
       <c r="C133" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>Glenn Maxwell</v>
+        <v>Deepak Chahar</v>
       </c>
       <c r="B134" t="str">
-        <v>RCB</v>
+        <v>CSK</v>
       </c>
       <c r="C134" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Romario Shepherd</v>
+        <v>Matt Henry</v>
       </c>
       <c r="B135" t="str">
-        <v>MI</v>
+        <v>LSG</v>
       </c>
       <c r="C135" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>Marco Jansen</v>
+        <v>Glenn Maxwell</v>
       </c>
       <c r="B136" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C136" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Wriddhiman Saha</v>
+        <v>Romario Shepherd</v>
       </c>
       <c r="B137" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C137" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Kane Williamson</v>
+        <v>Marco Jansen</v>
       </c>
       <c r="B138" t="str">
-        <v>GT</v>
+        <v>SRH</v>
       </c>
       <c r="C138" t="str">
         <v>0</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Chris Woakes</v>
+        <v>Mitchell Marsh</v>
       </c>
       <c r="B139" t="str">
-        <v>PBKS</v>
+        <v>DC</v>
       </c>
       <c r="C139" t="str">
         <v>0</v>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Dilshan Madushanka</v>
+        <v>Cameron Green</v>
       </c>
       <c r="B140" t="str">
-        <v>MI</v>
+        <v>RCB</v>
       </c>
       <c r="C140" t="str">
         <v>0</v>
@@ -1922,10 +1922,10 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>Nathan Ellis</v>
+        <v>Rahmanullah Gurbaz</v>
       </c>
       <c r="B141" t="str">
-        <v>PBKS</v>
+        <v>KKR</v>
       </c>
       <c r="C141" t="str">
         <v>0</v>
@@ -1933,10 +1933,10 @@
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>Navdeep Saini</v>
+        <v>Wriddhiman Saha</v>
       </c>
       <c r="B142" t="str">
-        <v>RR</v>
+        <v>GT</v>
       </c>
       <c r="C142" t="str">
         <v>0</v>
@@ -1944,10 +1944,10 @@
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>Mukesh Choudhary</v>
+        <v>Kane Williamson</v>
       </c>
       <c r="B143" t="str">
-        <v>CSK</v>
+        <v>GT</v>
       </c>
       <c r="C143" t="str">
         <v>0</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>Lalit Yadav</v>
+        <v>Chris Woakes</v>
       </c>
       <c r="B144" t="str">
-        <v>DC</v>
+        <v>PBKS</v>
       </c>
       <c r="C144" t="str">
         <v>0</v>
@@ -1966,10 +1966,10 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>Alzarri Joseph</v>
+        <v>Dilshan Madushanka</v>
       </c>
       <c r="B145" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C145" t="str">
         <v>0</v>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>Mitchell Marsh</v>
+        <v>Nathan Ellis</v>
       </c>
       <c r="B146" t="str">
-        <v>DC</v>
+        <v>PBKS</v>
       </c>
       <c r="C146" t="str">
         <v>0</v>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>Luke Wood</v>
+        <v>Mukesh Choudhary</v>
       </c>
       <c r="B147" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C147" t="str">
         <v>0</v>
@@ -1999,10 +1999,10 @@
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>Lizaad Williams</v>
+        <v>Navdeep Saini</v>
       </c>
       <c r="B148" t="str">
-        <v>DC</v>
+        <v>RR</v>
       </c>
       <c r="C148" t="str">
         <v>0</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Fazal Haque</v>
+        <v>Alzarri Joseph</v>
       </c>
       <c r="B149" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C149" t="str">
         <v>0</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>Mitchell Santner</v>
+        <v>Luke Wood</v>
       </c>
       <c r="B150" t="str">
-        <v>CSK</v>
+        <v>MI</v>
       </c>
       <c r="C150" t="str">
         <v>0</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>Krishnappa Gowtham</v>
+        <v>Lizaad Williams</v>
       </c>
       <c r="B151" t="str">
-        <v>LSG</v>
+        <v>DC</v>
       </c>
       <c r="C151" t="str">
         <v>0</v>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>Kyle Mayers</v>
+        <v>Fazal Haque</v>
       </c>
       <c r="B152" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C152" t="str">
         <v>0</v>
@@ -2054,10 +2054,10 @@
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>Nehal Wadhera</v>
+        <v>Mitchell Santner</v>
       </c>
       <c r="B153" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C153" t="str">
         <v>0</v>
@@ -2065,10 +2065,10 @@
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>Kumar Kushagra</v>
+        <v>Krishnappa Gowtham</v>
       </c>
       <c r="B154" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C154" t="str">
         <v>0</v>
@@ -2076,21 +2076,21 @@
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>Amit Mishra</v>
+        <v>Matthew Wade</v>
       </c>
       <c r="B155" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C155" t="str">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>Sai Kishore</v>
+        <v>Kyle Mayers</v>
       </c>
       <c r="B156" t="str">
-        <v>GT</v>
+        <v>LSG</v>
       </c>
       <c r="C156" t="str">
         <v>0</v>
@@ -2098,10 +2098,10 @@
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>Suyash Prabhudessai</v>
+        <v>Nehal Wadhera</v>
       </c>
       <c r="B157" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C157" t="str">
         <v>0</v>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>Washington Sundar</v>
+        <v>Kumar Kushagra</v>
       </c>
       <c r="B158" t="str">
-        <v>SRH</v>
+        <v>DC</v>
       </c>
       <c r="C158" t="str">
         <v>0</v>
@@ -2120,10 +2120,10 @@
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>Anrich Nortje</v>
+        <v>Amit Mishra</v>
       </c>
       <c r="B159" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C159" t="str">
         <v>0</v>
@@ -2131,10 +2131,10 @@
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>Manish Pandey</v>
+        <v>Suyash Prabhudessai</v>
       </c>
       <c r="B160" t="str">
-        <v>KKR</v>
+        <v>RCB</v>
       </c>
       <c r="C160" t="str">
         <v>0</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>Karn Sharma</v>
+        <v>Sai Kishore</v>
       </c>
       <c r="B161" t="str">
-        <v>RCB</v>
+        <v>GT</v>
       </c>
       <c r="C161" t="str">
         <v>0</v>
@@ -2153,10 +2153,10 @@
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>Sandeep Sharma</v>
+        <v>Suyash Sharma</v>
       </c>
       <c r="B162" t="str">
-        <v>RR</v>
+        <v>KKR</v>
       </c>
       <c r="C162" t="str">
         <v>0</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>Yash Dhull</v>
+        <v>Karn Sharma</v>
       </c>
       <c r="B163" t="str">
-        <v>DC</v>
+        <v>RCB</v>
       </c>
       <c r="C163" t="str">
         <v>0</v>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>Umran Malik</v>
+        <v>Sandeep Sharma</v>
       </c>
       <c r="B164" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C164" t="str">
         <v>0</v>
@@ -2186,10 +2186,10 @@
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>Nitish Rana</v>
+        <v>Yash Dhull</v>
       </c>
       <c r="B165" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C165" t="str">
         <v>0</v>
@@ -2197,10 +2197,10 @@
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>Azmatullah Omarzai</v>
+        <v>Manish Pandey</v>
       </c>
       <c r="B166" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C166" t="str">
         <v>0</v>
@@ -2208,10 +2208,10 @@
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>Rahul Chahar</v>
+        <v>Umran Malik</v>
       </c>
       <c r="B167" t="str">
-        <v>PBKS</v>
+        <v>SRH</v>
       </c>
       <c r="C167" t="str">
         <v>0</v>
@@ -2219,10 +2219,10 @@
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>Kwena Maphaka</v>
+        <v>Azmatullah Omarzai</v>
       </c>
       <c r="B168" t="str">
-        <v>MI</v>
+        <v>GT</v>
       </c>
       <c r="C168" t="str">
         <v>0</v>
@@ -2230,10 +2230,10 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Keshav Maharaj</v>
+        <v>Nitish Rana</v>
       </c>
       <c r="B169" t="str">
-        <v>RR</v>
+        <v>KKR</v>
       </c>
       <c r="C169" t="str">
         <v>0</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Dushmantha Chameera</v>
+        <v>Rahul Chahar</v>
       </c>
       <c r="B170" t="str">
-        <v>KKR</v>
+        <v>PBKS</v>
       </c>
       <c r="C170" t="str">
         <v>0</v>
@@ -2252,10 +2252,10 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Manav Suthar</v>
+        <v>Keshav Maharaj</v>
       </c>
       <c r="B171" t="str">
-        <v>GT</v>
+        <v>RR</v>
       </c>
       <c r="C171" t="str">
         <v>0</v>
@@ -2263,10 +2263,10 @@
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>Praveen Dubey</v>
+        <v>Dushmantha Chameera</v>
       </c>
       <c r="B172" t="str">
-        <v>DC</v>
+        <v>KKR</v>
       </c>
       <c r="C172" t="str">
         <v>0</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>Arjun Tendulkar</v>
+        <v>Kwena Maphaka</v>
       </c>
       <c r="B173" t="str">
         <v>MI</v>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>Cameron Green</v>
+        <v>Manav Suthar</v>
       </c>
       <c r="B174" t="str">
-        <v>RCB</v>
+        <v>GT</v>
       </c>
       <c r="C174" t="str">
         <v>0</v>
@@ -2296,10 +2296,10 @@
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>Rahmanullah Gurbaz</v>
+        <v>Jhye Richardson</v>
       </c>
       <c r="B175" t="str">
-        <v>KKR</v>
+        <v>DC</v>
       </c>
       <c r="C175" t="str">
         <v>0</v>
@@ -2307,10 +2307,10 @@
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>Suyash Sharma</v>
+        <v>Arjun Tendulkar</v>
       </c>
       <c r="B176" t="str">
-        <v>KKR</v>
+        <v>MI</v>
       </c>
       <c r="C176" t="str">
         <v>0</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>Jhye Richardson</v>
+        <v>Rishi Dhawan</v>
       </c>
       <c r="B177" t="str">
-        <v>DC</v>
+        <v>PBKS</v>
       </c>
       <c r="C177" t="str">
         <v>0</v>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>Rishi Dhawan</v>
+        <v>Jason Behrendorff</v>
       </c>
       <c r="B178" t="str">
-        <v>PBKS</v>
+        <v>MI</v>
       </c>
       <c r="C178" t="str">
         <v>0</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>Simarjeet Singh</v>
+        <v>Praveen Dubey</v>
       </c>
       <c r="B180" t="str">
-        <v>CSK</v>
+        <v>DC</v>
       </c>
       <c r="C180" t="str">
         <v>0</v>
@@ -2362,10 +2362,10 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>Jason Behrendorff</v>
+        <v>Simarjeet Singh</v>
       </c>
       <c r="B181" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C181" t="str">
         <v>0</v>
@@ -2373,10 +2373,10 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>Donavon Ferreira</v>
+        <v>Sherfane Rutherford</v>
       </c>
       <c r="B182" t="str">
-        <v>RR</v>
+        <v>KKR</v>
       </c>
       <c r="C182" t="str">
         <v>0</v>
@@ -2384,10 +2384,10 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>Sherfane Rutherford</v>
+        <v>Tom Kohler-Cadmore</v>
       </c>
       <c r="B183" t="str">
-        <v>KKR</v>
+        <v>RR</v>
       </c>
       <c r="C183" t="str">
         <v>0</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>Tom Kohler-Cadmore</v>
+        <v>Donavon Ferreira</v>
       </c>
       <c r="B184" t="str">
         <v>RR</v>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>Glenn Phillips</v>
+        <v>Kunal Singh Rathore</v>
       </c>
       <c r="B186" t="str">
-        <v>SRH</v>
+        <v>RR</v>
       </c>
       <c r="C186" t="str">
         <v>0</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>Kunal Singh Rathore</v>
+        <v>SK Rasheed</v>
       </c>
       <c r="B187" t="str">
-        <v>RR</v>
+        <v>CSK</v>
       </c>
       <c r="C187" t="str">
         <v>0</v>
@@ -2439,10 +2439,10 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>Swastik Chikara</v>
+        <v>M Siddharth</v>
       </c>
       <c r="B188" t="str">
-        <v>DC</v>
+        <v>LSG</v>
       </c>
       <c r="C188" t="str">
         <v>0</v>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>Mayank Dagar</v>
+        <v>Swastik Chikara</v>
       </c>
       <c r="B189" t="str">
-        <v>RCB</v>
+        <v>DC</v>
       </c>
       <c r="C189" t="str">
         <v>0</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="190">
       <c r="A190" t="str">
-        <v>Mayank Agarwal</v>
+        <v>Mayank Dagar</v>
       </c>
       <c r="B190" t="str">
-        <v>SRH</v>
+        <v>RCB</v>
       </c>
       <c r="C190" t="str">
         <v>0</v>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="191">
       <c r="A191" t="str">
-        <v>M Siddharth</v>
+        <v>Glenn Phillips</v>
       </c>
       <c r="B191" t="str">
-        <v>LSG</v>
+        <v>SRH</v>
       </c>
       <c r="C191" t="str">
         <v>0</v>
@@ -2483,10 +2483,10 @@
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>SK Rasheed</v>
+        <v>Allah Ghazanfar</v>
       </c>
       <c r="B192" t="str">
-        <v>CSK</v>
+        <v>KKR</v>
       </c>
       <c r="C192" t="str">
         <v>0</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>Piyush Chawla</v>
+        <v>Mayank Agarwal</v>
       </c>
       <c r="B193" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C193" t="str">
         <v>0</v>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="194">
       <c r="A194" t="str">
-        <v>Allah Ghazanfar</v>
+        <v>Harvik Desai</v>
       </c>
       <c r="B194" t="str">
-        <v>KKR</v>
+        <v>MI</v>
       </c>
       <c r="C194" t="str">
         <v>0</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="195">
       <c r="A195" t="str">
-        <v>Harvik Desai</v>
+        <v>BR sharath</v>
       </c>
       <c r="B195" t="str">
-        <v>MI</v>
+        <v>GT</v>
       </c>
       <c r="C195" t="str">
         <v>0</v>
@@ -2527,10 +2527,10 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Sandeep Warrier</v>
+        <v>Piyush Chawla</v>
       </c>
       <c r="B196" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C196" t="str">
         <v>0</v>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>BR sharath</v>
+        <v>Anshul Kamboj</v>
       </c>
       <c r="B197" t="str">
-        <v>GT</v>
+        <v>MI</v>
       </c>
       <c r="C197" t="str">
         <v>0</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>Tanay Thyagarajan</v>
+        <v>Ashton Turner</v>
       </c>
       <c r="B198" t="str">
-        <v>PBKS</v>
+        <v>LSG</v>
       </c>
       <c r="C198" t="str">
         <v>0</v>
@@ -2560,10 +2560,10 @@
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>Anshul Kamboj</v>
+        <v>Ajay Mandal</v>
       </c>
       <c r="B199" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C199" t="str">
         <v>0</v>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Ajay Mandal</v>
+        <v>Shivalik Sharma</v>
       </c>
       <c r="B200" t="str">
-        <v>CSK</v>
+        <v>MI</v>
       </c>
       <c r="C200" t="str">
         <v>0</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Shivalik Sharma</v>
+        <v>Shams Mulani</v>
       </c>
       <c r="B201" t="str">
         <v>MI</v>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Ashton Turner</v>
+        <v>Sandeep Warrier</v>
       </c>
       <c r="B202" t="str">
-        <v>LSG</v>
+        <v>GT</v>
       </c>
       <c r="C202" t="str">
         <v>0</v>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Nishant Sindhu</v>
+        <v>Tanay Thyagarajan</v>
       </c>
       <c r="B203" t="str">
-        <v>CSK</v>
+        <v>PBKS</v>
       </c>
       <c r="C203" t="str">
         <v>0</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Yudhvir Singh</v>
+        <v>Arshin Kulkarni</v>
       </c>
       <c r="B205" t="str">
         <v>LSG</v>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Shams Mulani</v>
+        <v>Nishant Sindhu</v>
       </c>
       <c r="B206" t="str">
-        <v>MI</v>
+        <v>CSK</v>
       </c>
       <c r="C206" t="str">
         <v>0</v>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Arshin Kulkarni</v>
+        <v>Manoj Bhandage</v>
       </c>
       <c r="B207" t="str">
-        <v>LSG</v>
+        <v>RCB</v>
       </c>
       <c r="C207" t="str">
         <v>0</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>Manoj Bhandage</v>
+        <v>Swapnil Singh</v>
       </c>
       <c r="B209" t="str">
         <v>RCB</v>
@@ -2681,10 +2681,10 @@
     </row>
     <row r="210">
       <c r="A210" t="str">
-        <v>Swapnil Singh</v>
+        <v>Vishwapratap Singh</v>
       </c>
       <c r="B210" t="str">
-        <v>RCB</v>
+        <v>PBKS</v>
       </c>
       <c r="C210" t="str">
         <v>0</v>
@@ -2692,10 +2692,10 @@
     </row>
     <row r="211">
       <c r="A211" t="str">
-        <v>Sanvir Singh</v>
+        <v>Rasikh Dar</v>
       </c>
       <c r="B211" t="str">
-        <v>SRH</v>
+        <v>DC</v>
       </c>
       <c r="C211" t="str">
         <v>0</v>
@@ -2703,10 +2703,10 @@
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>Vicky Ostwal</v>
+        <v>Joshua Little</v>
       </c>
       <c r="B212" t="str">
-        <v>DC</v>
+        <v>GT</v>
       </c>
       <c r="C212" t="str">
         <v>0</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>Rasikh Dar</v>
+        <v>Prashant Solanki</v>
       </c>
       <c r="B213" t="str">
-        <v>DC</v>
+        <v>CSK</v>
       </c>
       <c r="C213" t="str">
         <v>0</v>
@@ -2725,10 +2725,10 @@
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>Prashant Solanki</v>
+        <v>Sanvir Singh</v>
       </c>
       <c r="B214" t="str">
-        <v>CSK</v>
+        <v>SRH</v>
       </c>
       <c r="C214" t="str">
         <v>0</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="215">
       <c r="A215" t="str">
-        <v>Vishwapratap Singh</v>
+        <v>Vicky Ostwal</v>
       </c>
       <c r="B215" t="str">
-        <v>PBKS</v>
+        <v>DC</v>
       </c>
       <c r="C215" t="str">
         <v>0</v>
@@ -2747,10 +2747,10 @@
     </row>
     <row r="216">
       <c r="A216" t="str">
-        <v>Joshua Little</v>
+        <v>Chetan Sakariya</v>
       </c>
       <c r="B216" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C216" t="str">
         <v>0</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="217">
       <c r="A217" t="str">
-        <v>Jayant Yadav</v>
+        <v>Sushant Mishra</v>
       </c>
       <c r="B217" t="str">
         <v>GT</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>Sushant Mishra</v>
+        <v>Kartik Tyagi</v>
       </c>
       <c r="B218" t="str">
         <v>GT</v>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="219">
       <c r="A219" t="str">
-        <v>Chetan Sakariya</v>
+        <v>Jayant Yadav</v>
       </c>
       <c r="B219" t="str">
-        <v>KKR</v>
+        <v>GT</v>
       </c>
       <c r="C219" t="str">
         <v>0</v>
@@ -2802,10 +2802,10 @@
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>Kartik Tyagi</v>
+        <v>Vidhwath Kaverappa</v>
       </c>
       <c r="B221" t="str">
-        <v>GT</v>
+        <v>PBKS</v>
       </c>
       <c r="C221" t="str">
         <v>0</v>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>Vidhwath Kaverappa</v>
+        <v>Prince Choudhary</v>
       </c>
       <c r="B222" t="str">
         <v>PBKS</v>
@@ -2824,10 +2824,10 @@
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>Tom Curran</v>
+        <v>Nuwan Thushara</v>
       </c>
       <c r="B223" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C223" t="str">
         <v>0</v>
@@ -2835,10 +2835,10 @@
     </row>
     <row r="224">
       <c r="A224" t="str">
-        <v>Prince Choudhary</v>
+        <v>Yudhvir Singh</v>
       </c>
       <c r="B224" t="str">
-        <v>PBKS</v>
+        <v>LSG</v>
       </c>
       <c r="C224" t="str">
         <v>0</v>
@@ -2846,10 +2846,10 @@
     </row>
     <row r="225">
       <c r="A225" t="str">
-        <v>Abid Mushtaq</v>
+        <v>Akash Singh</v>
       </c>
       <c r="B225" t="str">
-        <v>RR</v>
+        <v>SRH</v>
       </c>
       <c r="C225" t="str">
         <v>0</v>
@@ -2857,10 +2857,10 @@
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>Akash Singh</v>
+        <v>Rajvardhan Hangargekar</v>
       </c>
       <c r="B226" t="str">
-        <v>SRH</v>
+        <v>CSK</v>
       </c>
       <c r="C226" t="str">
         <v>0</v>
@@ -2868,10 +2868,10 @@
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>Rajvardhan Hangargekar</v>
+        <v>Rajan Kumar</v>
       </c>
       <c r="B227" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C227" t="str">
         <v>0</v>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>Rajan Kumar</v>
+        <v>Ricky Bhui</v>
       </c>
       <c r="B228" t="str">
-        <v>RCB</v>
+        <v>DC</v>
       </c>
       <c r="C228" t="str">
         <v>0</v>
@@ -2890,10 +2890,10 @@
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>Himanshu Sharma</v>
+        <v>Aravelly Avanish</v>
       </c>
       <c r="B229" t="str">
-        <v>RCB</v>
+        <v>CSK</v>
       </c>
       <c r="C229" t="str">
         <v>0</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="230">
       <c r="A230" t="str">
-        <v>Aravelly Avanish</v>
+        <v>Tom Curran</v>
       </c>
       <c r="B230" t="str">
-        <v>CSK</v>
+        <v>RCB</v>
       </c>
       <c r="C230" t="str">
         <v>0</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="231">
       <c r="A231" t="str">
-        <v>Shivam Singh</v>
+        <v>Abid Mushtaq</v>
       </c>
       <c r="B231" t="str">
-        <v>PBKS</v>
+        <v>RR</v>
       </c>
       <c r="C231" t="str">
         <v>0</v>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>Anmolpreet Singh</v>
+        <v>Shivam Singh</v>
       </c>
       <c r="B232" t="str">
-        <v>SRH</v>
+        <v>PBKS</v>
       </c>
       <c r="C232" t="str">
         <v>0</v>
@@ -2934,7 +2934,7 @@
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>Upendra Yadav</v>
+        <v>Anmolpreet Singh</v>
       </c>
       <c r="B233" t="str">
         <v>SRH</v>
@@ -2945,10 +2945,10 @@
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>Ricky Bhui</v>
+        <v>Himanshu Sharma</v>
       </c>
       <c r="B234" t="str">
-        <v>DC</v>
+        <v>RCB</v>
       </c>
       <c r="C234" t="str">
         <v>0</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="235">
       <c r="A235" t="str">
-        <v>Kumar Kartikeya</v>
+        <v>Upendra Yadav</v>
       </c>
       <c r="B235" t="str">
-        <v>MI</v>
+        <v>SRH</v>
       </c>
       <c r="C235" t="str">
         <v>0</v>
@@ -2967,10 +2967,10 @@
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>Nuwan Thushara</v>
+        <v>Darshan Nalkande</v>
       </c>
       <c r="B236" t="str">
-        <v>MI</v>
+        <v>GT</v>
       </c>
       <c r="C236" t="str">
         <v>0</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="237">
       <c r="A237" t="str">
-        <v>Naman Dhir</v>
+        <v>Vishnu Vinod</v>
       </c>
       <c r="B237" t="str">
         <v>MI</v>
@@ -2989,10 +2989,10 @@
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>Darshan Nalkande</v>
+        <v>Srikar Bharat</v>
       </c>
       <c r="B238" t="str">
-        <v>GT</v>
+        <v>KKR</v>
       </c>
       <c r="C238" t="str">
         <v>0</v>
@@ -3000,10 +3000,10 @@
     </row>
     <row r="239">
       <c r="A239" t="str">
-        <v>Vishnu Vinod</v>
+        <v>Shubham Dubey</v>
       </c>
       <c r="B239" t="str">
-        <v>MI</v>
+        <v>RR</v>
       </c>
       <c r="C239" t="str">
         <v>0</v>
@@ -3011,10 +3011,10 @@
     </row>
     <row r="240">
       <c r="A240" t="str">
-        <v>Srikar Bharat</v>
+        <v>Nandre Burger</v>
       </c>
       <c r="B240" t="str">
-        <v>KKR</v>
+        <v>RR</v>
       </c>
       <c r="C240" t="str">
         <v>0</v>
@@ -3022,10 +3022,10 @@
     </row>
     <row r="241">
       <c r="A241" t="str">
-        <v>Shubham Dubey</v>
+        <v>Mayank Yadav</v>
       </c>
       <c r="B241" t="str">
-        <v>RR</v>
+        <v>LSG</v>
       </c>
       <c r="C241" t="str">
         <v>0</v>
@@ -3033,21 +3033,21 @@
     </row>
     <row r="242">
       <c r="A242" t="str">
-        <v>Nandre Burger</v>
+        <v>Mohammed Siraj</v>
       </c>
       <c r="B242" t="str">
-        <v>RR</v>
+        <v>RCB</v>
       </c>
       <c r="C242" t="str">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
-        <v>Mayank Yadav</v>
+        <v>Kumar Kartikeya</v>
       </c>
       <c r="B243" t="str">
-        <v>LSG</v>
+        <v>MI</v>
       </c>
       <c r="C243" t="str">
         <v>0</v>
@@ -3055,18 +3055,18 @@
     </row>
     <row r="244">
       <c r="A244" t="str">
-        <v>Yash Dayal</v>
+        <v>Naman Dhir</v>
       </c>
       <c r="B244" t="str">
-        <v>RCB</v>
+        <v>MI</v>
       </c>
       <c r="C244" t="str">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
-        <v>Mohammed Siraj</v>
+        <v>Yash Dayal</v>
       </c>
       <c r="B245" t="str">
         <v>RCB</v>

</xml_diff>